<commit_message>
added data via mysql
</commit_message>
<xml_diff>
--- a/app/resources/sqldata/ingredientsTable.xlsx
+++ b/app/resources/sqldata/ingredientsTable.xlsx
@@ -424,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>